<commit_message>
ITEM - eviolite work
documentation on implementing eviolite item functions including calculating a mon's BST
</commit_message>
<xml_diff>
--- a/hoenn isles/Documentation.xlsx
+++ b/hoenn isles/Documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" firstSheet="2" activeTab="3" xr2:uid="{088997C0-4E52-4395-A26A-BD7124426C35}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" firstSheet="2" activeTab="6" xr2:uid="{088997C0-4E52-4395-A26A-BD7124426C35}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -877,7 +877,7 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -1161,7 +1161,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New types added (graphical glitches)
</commit_message>
<xml_diff>
--- a/hoenn isles/Documentation.xlsx
+++ b/hoenn isles/Documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" firstSheet="2" activeTab="6" xr2:uid="{088997C0-4E52-4395-A26A-BD7124426C35}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" firstSheet="2" activeTab="4" xr2:uid="{088997C0-4E52-4395-A26A-BD7124426C35}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -1011,7 +1011,7 @@
   </sheetPr>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1240,7 +1240,7 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
type boosting items done
</commit_message>
<xml_diff>
--- a/hoenn isles/Documentation.xlsx
+++ b/hoenn isles/Documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" firstSheet="2" activeTab="4" xr2:uid="{088997C0-4E52-4395-A26A-BD7124426C35}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" firstSheet="2" activeTab="6" xr2:uid="{088997C0-4E52-4395-A26A-BD7124426C35}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>This is a theory and needs to be tested and verified</t>
   </si>
   <si>
-    <t>Open src/pokemon/pokemon_data.c</t>
-  </si>
-  <si>
     <t>Find the structure "gHoldEffectToType"</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>Add other things such as declarations and includes that may be required (like evolve with status condition, for example)</t>
+  </si>
+  <si>
+    <t>Open src/battle/calculate_base_damage.c</t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,7 @@
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -685,13 +685,13 @@
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -717,17 +717,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -759,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -783,17 +783,17 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -820,12 +820,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -841,12 +841,12 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -888,12 +888,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -909,12 +909,12 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,12 +922,12 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -935,12 +935,12 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -948,12 +948,12 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -961,12 +961,12 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -974,12 +974,12 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1011,7 +1011,7 @@
   </sheetPr>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1022,12 +1022,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1043,12 +1043,12 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1064,12 +1064,12 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1085,7 +1085,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1093,12 +1093,12 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1106,7 +1106,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1114,12 +1114,12 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1135,17 +1135,17 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1240,8 +1240,8 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1280,12 +1280,12 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1293,7 +1293,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1301,12 +1301,12 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1314,12 +1314,12 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>